<commit_message>
First Attempt for TM of eForm subtype 16, partial organization mapping
</commit_message>
<xml_diff>
--- a/mappings/package_cn_general/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_cn_general/transformation/conceptual_mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\valexande\work\repos\ted-rdf-mapping\mappings\package_cn_general\transformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12D1F6E-BFAD-44B1-981E-740475957216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0235988C-0425-4707-8B6D-3BB4469DCF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>Field</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>XML PATH Fragment</t>
+  </si>
+  <si>
+    <t>technical_mapping_es16.rml.ttl</t>
   </si>
 </sst>
 </file>
@@ -8661,7 +8664,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B3" sqref="B3"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -8678,7 +8681,9 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>61</v>
       </c>

</xml_diff>